<commit_message>
overhaul of figure order
</commit_message>
<xml_diff>
--- a/raw/cognition/raw_xlsx/V2 vs V3 - SPSS Template.xlsx
+++ b/raw/cognition/raw_xlsx/V2 vs V3 - SPSS Template.xlsx
@@ -21,12 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="98">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Visit</t>
+    <t xml:space="preserve">visit</t>
   </si>
   <si>
     <t xml:space="preserve">Coffee_Type</t>
@@ -200,6 +200,9 @@
     <t xml:space="preserve">APC115-008</t>
   </si>
   <si>
+    <t xml:space="preserve">V2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Coffee</t>
   </si>
   <si>
@@ -299,7 +302,13 @@
     <t xml:space="preserve">APC115-109</t>
   </si>
   <si>
+    <t xml:space="preserve">V3</t>
+  </si>
+  <si>
     <t xml:space="preserve">No Coffee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visit</t>
   </si>
   <si>
     <t xml:space="preserve">Time_point_CAR</t>
@@ -317,7 +326,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -345,12 +354,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -424,44 +427,44 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:BF63"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35:C63"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="1" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="7.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="8.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="9.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="17.28"/>
@@ -469,14 +472,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="18.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="14.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="17"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="25" style="2" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="31" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="25" style="2" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="31" style="1" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="34" style="0" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="50" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -659,11 +660,11 @@
       <c r="A2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>2</v>
+      <c r="B2" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3" t="n">
         <v>24.3</v>
@@ -833,13 +834,13 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="D3" s="3" t="n">
         <v>21.8479745106964</v>
@@ -1009,16 +1010,16 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>2</v>
+        <v>62</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>123</v>
@@ -1185,13 +1186,13 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>2</v>
+        <v>64</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D5" s="3" t="n">
         <v>30.5623016245727</v>
@@ -1361,13 +1362,13 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>2</v>
+        <v>65</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D6" s="3" t="n">
         <v>23.2115185950413</v>
@@ -1531,13 +1532,13 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>2</v>
+        <v>66</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D7" s="3" t="n">
         <v>26.5181861881109</v>
@@ -1707,13 +1708,13 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="2" t="n">
-        <v>2</v>
+        <v>67</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D8" s="3" t="n">
         <v>25.9094569517874</v>
@@ -1881,13 +1882,13 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" s="2" t="n">
-        <v>2</v>
+        <v>68</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D9" s="3" t="n">
         <v>24.4535684096124</v>
@@ -2055,13 +2056,13 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="2" t="n">
-        <v>2</v>
+        <v>69</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D10" s="3" t="n">
         <v>28.9965397923875</v>
@@ -2231,13 +2232,13 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" s="2" t="n">
-        <v>2</v>
+        <v>70</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D11" s="3" t="n">
         <v>20.1476828494103</v>
@@ -2407,13 +2408,13 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="2" t="n">
-        <v>2</v>
+        <v>71</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D12" s="3" t="n">
         <v>27.3511342155009</v>
@@ -2583,13 +2584,13 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="2" t="n">
-        <v>2</v>
+        <v>72</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D13" s="3" t="n">
         <v>24.5581208860971</v>
@@ -2759,13 +2760,13 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" s="2" t="n">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D14" s="3" t="n">
         <v>21.6071927783639</v>
@@ -2935,13 +2936,13 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" s="2" t="n">
-        <v>2</v>
+        <v>74</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D15" s="3" t="n">
         <v>25.0775510204082</v>
@@ -3105,13 +3106,13 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B16" s="2" t="n">
-        <v>2</v>
+        <v>75</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D16" s="3" t="n">
         <v>29.3946871824648</v>
@@ -3277,13 +3278,13 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B17" s="2" t="n">
-        <v>2</v>
+        <v>76</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D17" s="3" t="n">
         <v>26.1713444997737</v>
@@ -3449,13 +3450,13 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" s="2" t="n">
-        <v>2</v>
+        <v>77</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D18" s="3" t="n">
         <v>22.2</v>
@@ -3625,16 +3626,16 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B19" s="2" t="n">
-        <v>2</v>
+        <v>78</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E19" s="1" t="n">
         <v>128</v>
@@ -3801,13 +3802,13 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B20" s="2" t="n">
-        <v>2</v>
+        <v>80</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D20" s="3" t="n">
         <v>21.9921875</v>
@@ -3973,13 +3974,13 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B21" s="2" t="n">
-        <v>2</v>
+        <v>81</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D21" s="3" t="n">
         <v>21.6345270890725</v>
@@ -4149,13 +4150,13 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B22" s="2" t="n">
-        <v>2</v>
+        <v>82</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D22" s="3" t="n">
         <v>23.6081632653061</v>
@@ -4325,13 +4326,13 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B23" s="2" t="n">
-        <v>2</v>
+        <v>83</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D23" s="3" t="n">
         <v>24.7479912344777</v>
@@ -4499,13 +4500,13 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24" s="2" t="n">
-        <v>2</v>
+        <v>84</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D24" s="3" t="n">
         <v>21.3271604938272</v>
@@ -4675,13 +4676,13 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B25" s="2" t="n">
-        <v>2</v>
+        <v>85</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D25" s="3" t="n">
         <v>25.5789224952741</v>
@@ -4851,13 +4852,13 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B26" s="2" t="n">
-        <v>2</v>
+        <v>86</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D26" s="3" t="n">
         <v>20.6396358165194</v>
@@ -5027,13 +5028,13 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B27" s="2" t="n">
-        <v>2</v>
+        <v>87</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D27" s="3" t="n">
         <v>29.3221077079402</v>
@@ -5203,13 +5204,13 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B28" s="2" t="n">
-        <v>2</v>
+        <v>88</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D28" s="3" t="n">
         <v>26.2053857441048</v>
@@ -5379,13 +5380,13 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B29" s="2" t="n">
-        <v>2</v>
+        <v>89</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D29" s="3" t="n">
         <v>23.3843537414966</v>
@@ -5555,13 +5556,13 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B30" s="2" t="n">
-        <v>2</v>
+        <v>90</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D30" s="3" t="n">
         <v>19.6321491559587</v>
@@ -5727,13 +5728,13 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B31" s="2" t="n">
-        <v>2</v>
+        <v>91</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D31" s="3" t="n">
         <v>29.0253113198714</v>
@@ -5903,13 +5904,13 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B32" s="2" t="n">
-        <v>2</v>
+        <v>92</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D32" s="3" t="n">
         <v>27.8342284801858</v>
@@ -6067,11 +6068,11 @@
       <c r="A33" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="2" t="n">
-        <v>3</v>
+      <c r="B33" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D33" s="5" t="n">
         <v>24.0210502489814</v>
@@ -6241,13 +6242,13 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B34" s="2" t="n">
-        <v>3</v>
+        <v>61</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D34" s="5" t="n">
         <v>21.8129617310318</v>
@@ -6417,13 +6418,13 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B35" s="2" t="n">
-        <v>3</v>
+        <v>62</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D35" s="5" t="n">
         <v>20.7897153351699</v>
@@ -6593,13 +6594,13 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B36" s="2" t="n">
-        <v>3</v>
+        <v>64</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D36" s="5" t="n">
         <v>31.1213681177051</v>
@@ -6767,13 +6768,13 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B37" s="2" t="n">
-        <v>3</v>
+        <v>65</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D37" s="5" t="n">
         <v>23.4697830578512</v>
@@ -6937,13 +6938,13 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B38" s="2" t="n">
-        <v>3</v>
+        <v>66</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D38" s="5" t="n">
         <v>26.1176093574748</v>
@@ -7111,13 +7112,13 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B39" s="2" t="n">
-        <v>3</v>
+        <v>67</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D39" s="5" t="n">
         <v>26.3296103077623</v>
@@ -7281,13 +7282,13 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B40" s="2" t="n">
-        <v>3</v>
+        <v>68</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D40" s="5" t="n">
         <v>24.5441371814998</v>
@@ -7451,13 +7452,13 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B41" s="2" t="n">
-        <v>3</v>
+        <v>69</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D41" s="5" t="n">
         <v>29.3079584775087</v>
@@ -7627,13 +7628,13 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B42" s="2" t="n">
-        <v>3</v>
+        <v>70</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D42" s="5" t="n">
         <v>20.7156938086805</v>
@@ -7803,13 +7804,13 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B43" s="2" t="n">
-        <v>3</v>
+        <v>71</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D43" s="5" t="n">
         <v>26.5831758034026</v>
@@ -7979,13 +7980,13 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B44" s="2" t="n">
-        <v>3</v>
+        <v>72</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D44" s="5" t="n">
         <v>23.8898726987203</v>
@@ -8133,13 +8134,13 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B45" s="2" t="n">
-        <v>3</v>
+        <v>73</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D45" s="5" t="n">
         <v>21.2825438050663</v>
@@ -8309,13 +8310,13 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B46" s="2" t="n">
-        <v>3</v>
+        <v>74</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D46" s="6" t="n">
         <v>24.6530612244898</v>
@@ -8475,13 +8476,13 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B47" s="2" t="n">
-        <v>3</v>
+        <v>75</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D47" s="6" t="n">
         <v>29.2858179706779</v>
@@ -8651,13 +8652,13 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B48" s="2" t="n">
-        <v>3</v>
+        <v>76</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D48" s="6" t="n">
         <v>26.2845178813943</v>
@@ -8827,13 +8828,13 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B49" s="2" t="n">
-        <v>3</v>
+        <v>77</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D49" s="5" t="n">
         <v>22.7420402858999</v>
@@ -9003,13 +9004,13 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B50" s="2" t="n">
-        <v>3</v>
+        <v>78</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D50" s="5" t="n">
         <v>22.3289132754153</v>
@@ -9179,13 +9180,13 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B51" s="2" t="n">
-        <v>3</v>
+        <v>80</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D51" s="5" t="n">
         <v>21.8359375</v>
@@ -9337,13 +9338,13 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B52" s="2" t="n">
-        <v>3</v>
+        <v>81</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D52" s="5" t="n">
         <v>21.2304866850321</v>
@@ -9511,13 +9512,13 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B53" s="2" t="n">
-        <v>3</v>
+        <v>82</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D53" s="5" t="n">
         <v>23.3795918367347</v>
@@ -9685,13 +9686,13 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B54" s="2" t="n">
-        <v>3</v>
+        <v>83</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D54" s="5" t="n">
         <v>24.6603360116874</v>
@@ -9857,13 +9858,13 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B55" s="2" t="n">
-        <v>3</v>
+        <v>84</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D55" s="5" t="n">
         <v>21.3271604938272</v>
@@ -10029,13 +10030,13 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B56" s="2" t="n">
-        <v>3</v>
+        <v>85</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D56" s="5" t="n">
         <v>25.7561436672968</v>
@@ -10205,13 +10206,13 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B57" s="2" t="n">
-        <v>3</v>
+        <v>86</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D57" s="5" t="n">
         <v>20.6010570579839</v>
@@ -10381,13 +10382,13 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B58" s="2" t="n">
-        <v>3</v>
+        <v>87</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D58" s="5" t="n">
         <v>29.5035563942517</v>
@@ -10557,13 +10558,13 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B59" s="2" t="n">
-        <v>3</v>
+        <v>88</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D59" s="5" t="n">
         <v>26.177830133438</v>
@@ -10733,13 +10734,13 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B60" s="2" t="n">
-        <v>3</v>
+        <v>89</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D60" s="5" t="n">
         <v>22.6757369614513</v>
@@ -10909,13 +10910,13 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B61" s="2" t="n">
-        <v>3</v>
+        <v>90</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D61" s="6" t="n">
         <v>19.9546485260771</v>
@@ -11083,13 +11084,13 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B62" s="1" t="n">
-        <v>3</v>
+        <v>91</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D62" s="6" t="n">
         <v>28.9004712711838</v>
@@ -11259,13 +11260,13 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B63" s="1" t="n">
-        <v>3</v>
+        <v>92</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D63" s="6" t="n">
         <v>27.9430976919727</v>
@@ -11442,23 +11443,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D249"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G29" activeCellId="1" sqref="C35:C63 G29"/>
+      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.99"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11466,13 +11466,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11491,7 +11491,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>2</v>
@@ -11505,7 +11505,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>2</v>
@@ -11519,7 +11519,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>2</v>
@@ -11533,7 +11533,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>2</v>
@@ -11545,7 +11545,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>2</v>
@@ -11559,7 +11559,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>2</v>
@@ -11573,7 +11573,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>2</v>
@@ -11587,7 +11587,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>2</v>
@@ -11601,7 +11601,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>2</v>
@@ -11615,7 +11615,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>2</v>
@@ -11629,7 +11629,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>2</v>
@@ -11643,7 +11643,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B14" s="2" t="n">
         <v>2</v>
@@ -11657,7 +11657,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B15" s="2" t="n">
         <v>2</v>
@@ -11671,7 +11671,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B16" s="2" t="n">
         <v>2</v>
@@ -11685,7 +11685,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>2</v>
@@ -11699,7 +11699,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B18" s="2" t="n">
         <v>2</v>
@@ -11713,7 +11713,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B19" s="2" t="n">
         <v>2</v>
@@ -11727,7 +11727,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B20" s="2" t="n">
         <v>2</v>
@@ -11741,7 +11741,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B21" s="2" t="n">
         <v>2</v>
@@ -11755,7 +11755,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B22" s="2" t="n">
         <v>2</v>
@@ -11769,7 +11769,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B23" s="2" t="n">
         <v>2</v>
@@ -11783,7 +11783,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B24" s="2" t="n">
         <v>2</v>
@@ -11797,7 +11797,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B25" s="2" t="n">
         <v>2</v>
@@ -11811,7 +11811,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B26" s="2" t="n">
         <v>2</v>
@@ -11825,7 +11825,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B27" s="2" t="n">
         <v>2</v>
@@ -11839,7 +11839,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B28" s="2" t="n">
         <v>2</v>
@@ -11853,7 +11853,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B29" s="2" t="n">
         <v>2</v>
@@ -11867,7 +11867,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B30" s="2" t="n">
         <v>2</v>
@@ -11881,7 +11881,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B31" s="2" t="n">
         <v>2</v>
@@ -11895,7 +11895,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B32" s="2" t="n">
         <v>2</v>
@@ -11923,7 +11923,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B34" s="2" t="n">
         <v>3</v>
@@ -11937,7 +11937,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B35" s="2" t="n">
         <v>3</v>
@@ -11951,7 +11951,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B36" s="2" t="n">
         <v>3</v>
@@ -11965,7 +11965,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B37" s="2" t="n">
         <v>3</v>
@@ -11979,7 +11979,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B38" s="2" t="n">
         <v>3</v>
@@ -11993,7 +11993,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B39" s="2" t="n">
         <v>3</v>
@@ -12005,7 +12005,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B40" s="2" t="n">
         <v>3</v>
@@ -12019,7 +12019,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B41" s="2" t="n">
         <v>3</v>
@@ -12031,7 +12031,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B42" s="2" t="n">
         <v>3</v>
@@ -12045,7 +12045,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B43" s="2" t="n">
         <v>3</v>
@@ -12059,7 +12059,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B44" s="2" t="n">
         <v>3</v>
@@ -12073,7 +12073,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B45" s="2" t="n">
         <v>3</v>
@@ -12087,7 +12087,7 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B46" s="2" t="n">
         <v>3</v>
@@ -12101,7 +12101,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B47" s="2" t="n">
         <v>3</v>
@@ -12115,7 +12115,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B48" s="2" t="n">
         <v>3</v>
@@ -12129,7 +12129,7 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B49" s="2" t="n">
         <v>3</v>
@@ -12143,7 +12143,7 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B50" s="2" t="n">
         <v>3</v>
@@ -12157,7 +12157,7 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B51" s="2" t="n">
         <v>3</v>
@@ -12171,7 +12171,7 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B52" s="2" t="n">
         <v>3</v>
@@ -12185,7 +12185,7 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B53" s="2" t="n">
         <v>3</v>
@@ -12199,7 +12199,7 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B54" s="2" t="n">
         <v>3</v>
@@ -12213,7 +12213,7 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B55" s="2" t="n">
         <v>3</v>
@@ -12227,7 +12227,7 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B56" s="2" t="n">
         <v>3</v>
@@ -12241,7 +12241,7 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B57" s="2" t="n">
         <v>3</v>
@@ -12255,7 +12255,7 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B58" s="2" t="n">
         <v>3</v>
@@ -12269,7 +12269,7 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B59" s="2" t="n">
         <v>3</v>
@@ -12283,7 +12283,7 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B60" s="2" t="n">
         <v>3</v>
@@ -12297,7 +12297,7 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B61" s="2" t="n">
         <v>3</v>
@@ -12311,7 +12311,7 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B62" s="1" t="n">
         <v>3</v>
@@ -12325,7 +12325,7 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B63" s="1" t="n">
         <v>3</v>
@@ -12353,7 +12353,7 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B65" s="2" t="n">
         <v>2</v>
@@ -12367,7 +12367,7 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B66" s="2" t="n">
         <v>2</v>
@@ -12381,7 +12381,7 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B67" s="2" t="n">
         <v>2</v>
@@ -12395,7 +12395,7 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B68" s="2" t="n">
         <v>2</v>
@@ -12407,7 +12407,7 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B69" s="2" t="n">
         <v>2</v>
@@ -12421,7 +12421,7 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B70" s="2" t="n">
         <v>2</v>
@@ -12435,7 +12435,7 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B71" s="2" t="n">
         <v>2</v>
@@ -12449,7 +12449,7 @@
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B72" s="2" t="n">
         <v>2</v>
@@ -12463,7 +12463,7 @@
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B73" s="2" t="n">
         <v>2</v>
@@ -12477,7 +12477,7 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B74" s="2" t="n">
         <v>2</v>
@@ -12491,7 +12491,7 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B75" s="2" t="n">
         <v>2</v>
@@ -12505,7 +12505,7 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B76" s="2" t="n">
         <v>2</v>
@@ -12519,7 +12519,7 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B77" s="2" t="n">
         <v>2</v>
@@ -12533,7 +12533,7 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B78" s="2" t="n">
         <v>2</v>
@@ -12547,7 +12547,7 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B79" s="2" t="n">
         <v>2</v>
@@ -12561,7 +12561,7 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B80" s="2" t="n">
         <v>2</v>
@@ -12575,7 +12575,7 @@
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B81" s="2" t="n">
         <v>2</v>
@@ -12589,7 +12589,7 @@
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B82" s="2" t="n">
         <v>2</v>
@@ -12603,7 +12603,7 @@
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B83" s="2" t="n">
         <v>2</v>
@@ -12617,7 +12617,7 @@
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B84" s="2" t="n">
         <v>2</v>
@@ -12631,7 +12631,7 @@
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B85" s="2" t="n">
         <v>2</v>
@@ -12645,7 +12645,7 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B86" s="2" t="n">
         <v>2</v>
@@ -12659,7 +12659,7 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B87" s="2" t="n">
         <v>2</v>
@@ -12673,7 +12673,7 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B88" s="2" t="n">
         <v>2</v>
@@ -12687,7 +12687,7 @@
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B89" s="2" t="n">
         <v>2</v>
@@ -12701,7 +12701,7 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B90" s="2" t="n">
         <v>2</v>
@@ -12715,7 +12715,7 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B91" s="2" t="n">
         <v>2</v>
@@ -12729,7 +12729,7 @@
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B92" s="2" t="n">
         <v>2</v>
@@ -12743,7 +12743,7 @@
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B93" s="2" t="n">
         <v>2</v>
@@ -12757,7 +12757,7 @@
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B94" s="2" t="n">
         <v>2</v>
@@ -12785,7 +12785,7 @@
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B96" s="2" t="n">
         <v>3</v>
@@ -12799,7 +12799,7 @@
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B97" s="2" t="n">
         <v>3</v>
@@ -12813,7 +12813,7 @@
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B98" s="2" t="n">
         <v>3</v>
@@ -12827,7 +12827,7 @@
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B99" s="2" t="n">
         <v>3</v>
@@ -12841,7 +12841,7 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B100" s="2" t="n">
         <v>3</v>
@@ -12855,7 +12855,7 @@
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B101" s="2" t="n">
         <v>3</v>
@@ -12867,7 +12867,7 @@
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B102" s="2" t="n">
         <v>3</v>
@@ -12881,7 +12881,7 @@
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B103" s="2" t="n">
         <v>3</v>
@@ -12895,7 +12895,7 @@
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B104" s="2" t="n">
         <v>3</v>
@@ -12909,7 +12909,7 @@
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B105" s="2" t="n">
         <v>3</v>
@@ -12923,7 +12923,7 @@
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B106" s="2" t="n">
         <v>3</v>
@@ -12937,7 +12937,7 @@
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B107" s="2" t="n">
         <v>3</v>
@@ -12951,7 +12951,7 @@
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B108" s="2" t="n">
         <v>3</v>
@@ -12965,7 +12965,7 @@
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B109" s="2" t="n">
         <v>3</v>
@@ -12979,7 +12979,7 @@
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B110" s="2" t="n">
         <v>3</v>
@@ -12993,7 +12993,7 @@
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B111" s="2" t="n">
         <v>3</v>
@@ -13007,7 +13007,7 @@
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B112" s="2" t="n">
         <v>3</v>
@@ -13021,7 +13021,7 @@
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B113" s="2" t="n">
         <v>3</v>
@@ -13035,7 +13035,7 @@
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B114" s="2" t="n">
         <v>3</v>
@@ -13049,7 +13049,7 @@
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B115" s="2" t="n">
         <v>3</v>
@@ -13063,7 +13063,7 @@
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B116" s="2" t="n">
         <v>3</v>
@@ -13077,7 +13077,7 @@
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B117" s="2" t="n">
         <v>3</v>
@@ -13091,7 +13091,7 @@
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B118" s="2" t="n">
         <v>3</v>
@@ -13105,7 +13105,7 @@
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B119" s="2" t="n">
         <v>3</v>
@@ -13119,7 +13119,7 @@
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B120" s="2" t="n">
         <v>3</v>
@@ -13133,7 +13133,7 @@
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B121" s="2" t="n">
         <v>3</v>
@@ -13147,7 +13147,7 @@
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B122" s="2" t="n">
         <v>3</v>
@@ -13161,7 +13161,7 @@
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B123" s="2" t="n">
         <v>3</v>
@@ -13175,7 +13175,7 @@
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B124" s="1" t="n">
         <v>3</v>
@@ -13189,7 +13189,7 @@
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B125" s="1" t="n">
         <v>3</v>
@@ -13217,7 +13217,7 @@
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B127" s="2" t="n">
         <v>2</v>
@@ -13231,7 +13231,7 @@
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B128" s="2" t="n">
         <v>2</v>
@@ -13245,7 +13245,7 @@
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B129" s="2" t="n">
         <v>2</v>
@@ -13259,7 +13259,7 @@
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B130" s="2" t="n">
         <v>2</v>
@@ -13271,7 +13271,7 @@
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B131" s="2" t="n">
         <v>2</v>
@@ -13285,7 +13285,7 @@
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B132" s="2" t="n">
         <v>2</v>
@@ -13299,7 +13299,7 @@
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B133" s="2" t="n">
         <v>2</v>
@@ -13313,7 +13313,7 @@
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B134" s="2" t="n">
         <v>2</v>
@@ -13327,7 +13327,7 @@
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B135" s="2" t="n">
         <v>2</v>
@@ -13341,7 +13341,7 @@
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B136" s="2" t="n">
         <v>2</v>
@@ -13355,7 +13355,7 @@
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B137" s="2" t="n">
         <v>2</v>
@@ -13369,7 +13369,7 @@
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B138" s="2" t="n">
         <v>2</v>
@@ -13383,7 +13383,7 @@
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B139" s="2" t="n">
         <v>2</v>
@@ -13397,7 +13397,7 @@
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B140" s="2" t="n">
         <v>2</v>
@@ -13411,7 +13411,7 @@
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B141" s="2" t="n">
         <v>2</v>
@@ -13425,7 +13425,7 @@
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B142" s="2" t="n">
         <v>2</v>
@@ -13439,7 +13439,7 @@
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B143" s="2" t="n">
         <v>2</v>
@@ -13453,7 +13453,7 @@
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B144" s="2" t="n">
         <v>2</v>
@@ -13467,7 +13467,7 @@
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B145" s="2" t="n">
         <v>2</v>
@@ -13481,7 +13481,7 @@
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B146" s="2" t="n">
         <v>2</v>
@@ -13495,7 +13495,7 @@
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B147" s="2" t="n">
         <v>2</v>
@@ -13509,7 +13509,7 @@
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B148" s="2" t="n">
         <v>2</v>
@@ -13523,7 +13523,7 @@
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B149" s="2" t="n">
         <v>2</v>
@@ -13537,7 +13537,7 @@
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B150" s="2" t="n">
         <v>2</v>
@@ -13551,7 +13551,7 @@
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B151" s="2" t="n">
         <v>2</v>
@@ -13565,7 +13565,7 @@
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B152" s="2" t="n">
         <v>2</v>
@@ -13579,7 +13579,7 @@
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B153" s="2" t="n">
         <v>2</v>
@@ -13593,7 +13593,7 @@
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B154" s="2" t="n">
         <v>2</v>
@@ -13607,7 +13607,7 @@
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B155" s="2" t="n">
         <v>2</v>
@@ -13621,7 +13621,7 @@
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B156" s="2" t="n">
         <v>2</v>
@@ -13649,7 +13649,7 @@
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B158" s="2" t="n">
         <v>3</v>
@@ -13663,7 +13663,7 @@
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B159" s="2" t="n">
         <v>3</v>
@@ -13677,7 +13677,7 @@
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B160" s="2" t="n">
         <v>3</v>
@@ -13691,7 +13691,7 @@
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B161" s="2" t="n">
         <v>3</v>
@@ -13705,7 +13705,7 @@
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B162" s="2" t="n">
         <v>3</v>
@@ -13719,7 +13719,7 @@
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B163" s="2" t="n">
         <v>3</v>
@@ -13731,7 +13731,7 @@
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B164" s="2" t="n">
         <v>3</v>
@@ -13745,7 +13745,7 @@
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B165" s="2" t="n">
         <v>3</v>
@@ -13759,7 +13759,7 @@
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B166" s="2" t="n">
         <v>3</v>
@@ -13773,7 +13773,7 @@
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B167" s="2" t="n">
         <v>3</v>
@@ -13787,7 +13787,7 @@
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B168" s="2" t="n">
         <v>3</v>
@@ -13801,7 +13801,7 @@
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B169" s="2" t="n">
         <v>3</v>
@@ -13815,7 +13815,7 @@
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B170" s="2" t="n">
         <v>3</v>
@@ -13829,7 +13829,7 @@
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B171" s="2" t="n">
         <v>3</v>
@@ -13843,7 +13843,7 @@
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B172" s="2" t="n">
         <v>3</v>
@@ -13857,7 +13857,7 @@
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B173" s="2" t="n">
         <v>3</v>
@@ -13871,7 +13871,7 @@
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B174" s="2" t="n">
         <v>3</v>
@@ -13885,7 +13885,7 @@
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B175" s="2" t="n">
         <v>3</v>
@@ -13899,7 +13899,7 @@
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B176" s="2" t="n">
         <v>3</v>
@@ -13913,7 +13913,7 @@
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B177" s="2" t="n">
         <v>3</v>
@@ -13927,7 +13927,7 @@
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B178" s="2" t="n">
         <v>3</v>
@@ -13941,7 +13941,7 @@
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B179" s="2" t="n">
         <v>3</v>
@@ -13955,7 +13955,7 @@
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B180" s="2" t="n">
         <v>3</v>
@@ -13969,7 +13969,7 @@
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B181" s="2" t="n">
         <v>3</v>
@@ -13983,7 +13983,7 @@
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B182" s="2" t="n">
         <v>3</v>
@@ -13997,7 +13997,7 @@
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B183" s="2" t="n">
         <v>3</v>
@@ -14011,7 +14011,7 @@
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B184" s="2" t="n">
         <v>3</v>
@@ -14025,7 +14025,7 @@
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B185" s="2" t="n">
         <v>3</v>
@@ -14039,7 +14039,7 @@
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B186" s="1" t="n">
         <v>3</v>
@@ -14053,7 +14053,7 @@
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B187" s="1" t="n">
         <v>3</v>
@@ -14081,7 +14081,7 @@
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B189" s="2" t="n">
         <v>2</v>
@@ -14093,7 +14093,7 @@
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B190" s="2" t="n">
         <v>2</v>
@@ -14107,7 +14107,7 @@
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B191" s="2" t="n">
         <v>2</v>
@@ -14121,7 +14121,7 @@
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B192" s="2" t="n">
         <v>2</v>
@@ -14133,7 +14133,7 @@
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B193" s="2" t="n">
         <v>2</v>
@@ -14147,7 +14147,7 @@
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B194" s="2" t="n">
         <v>2</v>
@@ -14161,7 +14161,7 @@
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B195" s="2" t="n">
         <v>2</v>
@@ -14175,7 +14175,7 @@
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B196" s="2" t="n">
         <v>2</v>
@@ -14189,7 +14189,7 @@
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B197" s="2" t="n">
         <v>2</v>
@@ -14203,7 +14203,7 @@
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B198" s="2" t="n">
         <v>2</v>
@@ -14217,7 +14217,7 @@
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B199" s="2" t="n">
         <v>2</v>
@@ -14231,7 +14231,7 @@
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B200" s="2" t="n">
         <v>2</v>
@@ -14245,7 +14245,7 @@
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B201" s="2" t="n">
         <v>2</v>
@@ -14259,7 +14259,7 @@
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B202" s="2" t="n">
         <v>2</v>
@@ -14273,7 +14273,7 @@
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B203" s="2" t="n">
         <v>2</v>
@@ -14287,7 +14287,7 @@
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B204" s="2" t="n">
         <v>2</v>
@@ -14301,7 +14301,7 @@
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B205" s="2" t="n">
         <v>2</v>
@@ -14315,7 +14315,7 @@
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B206" s="2" t="n">
         <v>2</v>
@@ -14329,7 +14329,7 @@
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B207" s="2" t="n">
         <v>2</v>
@@ -14343,7 +14343,7 @@
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B208" s="2" t="n">
         <v>2</v>
@@ -14357,7 +14357,7 @@
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B209" s="2" t="n">
         <v>2</v>
@@ -14371,7 +14371,7 @@
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B210" s="2" t="n">
         <v>2</v>
@@ -14385,7 +14385,7 @@
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B211" s="2" t="n">
         <v>2</v>
@@ -14399,7 +14399,7 @@
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B212" s="2" t="n">
         <v>2</v>
@@ -14413,7 +14413,7 @@
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B213" s="2" t="n">
         <v>2</v>
@@ -14427,7 +14427,7 @@
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B214" s="2" t="n">
         <v>2</v>
@@ -14441,7 +14441,7 @@
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B215" s="2" t="n">
         <v>2</v>
@@ -14455,7 +14455,7 @@
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B216" s="2" t="n">
         <v>2</v>
@@ -14469,7 +14469,7 @@
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B217" s="2" t="n">
         <v>2</v>
@@ -14483,7 +14483,7 @@
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B218" s="2" t="n">
         <v>2</v>
@@ -14511,7 +14511,7 @@
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B220" s="2" t="n">
         <v>3</v>
@@ -14525,7 +14525,7 @@
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B221" s="2" t="n">
         <v>3</v>
@@ -14539,7 +14539,7 @@
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B222" s="2" t="n">
         <v>3</v>
@@ -14553,7 +14553,7 @@
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B223" s="2" t="n">
         <v>3</v>
@@ -14567,7 +14567,7 @@
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B224" s="2" t="n">
         <v>3</v>
@@ -14581,7 +14581,7 @@
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B225" s="2" t="n">
         <v>3</v>
@@ -14593,7 +14593,7 @@
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B226" s="2" t="n">
         <v>3</v>
@@ -14607,7 +14607,7 @@
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B227" s="2" t="n">
         <v>3</v>
@@ -14621,7 +14621,7 @@
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B228" s="2" t="n">
         <v>3</v>
@@ -14635,7 +14635,7 @@
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B229" s="2" t="n">
         <v>3</v>
@@ -14649,7 +14649,7 @@
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B230" s="2" t="n">
         <v>3</v>
@@ -14663,7 +14663,7 @@
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B231" s="2" t="n">
         <v>3</v>
@@ -14677,7 +14677,7 @@
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B232" s="2" t="n">
         <v>3</v>
@@ -14691,7 +14691,7 @@
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B233" s="2" t="n">
         <v>3</v>
@@ -14705,7 +14705,7 @@
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B234" s="2" t="n">
         <v>3</v>
@@ -14719,7 +14719,7 @@
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B235" s="2" t="n">
         <v>3</v>
@@ -14733,7 +14733,7 @@
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B236" s="2" t="n">
         <v>3</v>
@@ -14747,7 +14747,7 @@
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B237" s="2" t="n">
         <v>3</v>
@@ -14761,7 +14761,7 @@
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B238" s="2" t="n">
         <v>3</v>
@@ -14775,7 +14775,7 @@
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B239" s="2" t="n">
         <v>3</v>
@@ -14789,7 +14789,7 @@
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B240" s="2" t="n">
         <v>3</v>
@@ -14803,7 +14803,7 @@
     </row>
     <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B241" s="2" t="n">
         <v>3</v>
@@ -14815,7 +14815,7 @@
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B242" s="2" t="n">
         <v>3</v>
@@ -14829,7 +14829,7 @@
     </row>
     <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B243" s="2" t="n">
         <v>3</v>
@@ -14843,7 +14843,7 @@
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B244" s="2" t="n">
         <v>3</v>
@@ -14857,7 +14857,7 @@
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B245" s="2" t="n">
         <v>3</v>
@@ -14871,7 +14871,7 @@
     </row>
     <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B246" s="2" t="n">
         <v>3</v>
@@ -14885,7 +14885,7 @@
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B247" s="2" t="n">
         <v>3</v>
@@ -14899,7 +14899,7 @@
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B248" s="1" t="n">
         <v>3</v>
@@ -14913,7 +14913,7 @@
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B249" s="1" t="n">
         <v>3</v>

</xml_diff>